<commit_message>
added few more tests
</commit_message>
<xml_diff>
--- a/AcronisTestCases.xlsx
+++ b/AcronisTestCases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Win10\PycharmProjects\pythonProject\acronisHomework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Win10\Documents\GitHub\AcronisHomework\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="48">
   <si>
     <t>/types, .zip file, empty name -&gt; get 404, { status: file name empty}</t>
   </si>
   <si>
-    <t>/types, non-existing file type, (e.g. some_file.ksksksk) -&gt; get 404 status file type not found??</t>
-  </si>
-  <si>
     <t>/types .ppt file, empty file</t>
   </si>
   <si>
@@ -44,9 +41,6 @@
     <t>/types, .exe file, file is empty -&gt; get 200, { status: file uploaded}</t>
   </si>
   <si>
-    <t>/types, file name contains special chars</t>
-  </si>
-  <si>
     <t>/types, file is very large (&gt; 1gB) -&gt; get some TooBigFile error?</t>
   </si>
   <si>
@@ -74,9 +68,6 @@
     <t>/scans/history, make sure there is at least one clean and one infected file -&gt; get 200 with status: [{ fileId: "123", status: "clean" }, { fileId: "456", status: "infected" }]</t>
   </si>
   <si>
-    <t>/scans/update, then /scan/history -&gt; scan history not affected by definitions update</t>
-  </si>
-  <si>
     <t>/scans/update, then scan clean file -&gt; verify scan functionality remains the same after updating definitions</t>
   </si>
   <si>
@@ -141,6 +132,42 @@
   </si>
   <si>
     <t>/types, .txt file, proper name -&gt; get 200, { status: clean}</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>/types, .cmd file, clean file -&gt; get 200 {status: clean}</t>
+  </si>
+  <si>
+    <t>/types, .js file, infected file -&gt; get 200, { status: file uploaded}</t>
+  </si>
+  <si>
+    <t>/types, .tar file, clean file -&gt; get 200, { status: file uploaded}</t>
+  </si>
+  <si>
+    <t>/types, file name contains special chars -&gt; get 400 {status: forbidden}</t>
+  </si>
+  <si>
+    <t>/scan/history, then scan clean file, /scan/history again -&gt; verify history updated with new entry: clean file</t>
+  </si>
+  <si>
+    <t>/scan/history, then scan infected file, /scan/history again -&gt; verify history updated with new entry: infected file</t>
+  </si>
+  <si>
+    <t>XSS attack through url</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>/types, non-existing file type, (e.g. some_file.ksksksk) -&gt; get 400</t>
+  </si>
+  <si>
+    <t>scan clean file, upload file with same name but infected re-scan -&gt; history shows 2 files with different id's</t>
+  </si>
+  <si>
+    <t>/scan/history, /scans/update, then /scan/history -&gt; scan history not affected by definitions update</t>
   </si>
 </sst>
 </file>
@@ -470,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F32"/>
+  <dimension ref="B3:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -486,38 +513,44 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6">
+    <row r="3" spans="2:7">
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="2:6">
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:6">
+      <c r="G4" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -525,175 +558,172 @@
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" ht="27">
+      <c r="G5" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
       <c r="B6" s="1">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:6">
+      <c r="G6" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
       <c r="B7" s="1">
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="27">
       <c r="B8" s="1">
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="27">
       <c r="B9" s="1">
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="C10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="C11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="C12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="27">
+      <c r="B13" s="1">
+        <v>7</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="27">
-      <c r="B10" s="1">
+      <c r="D13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="27">
+      <c r="B14" s="1">
+        <v>8</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="1">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="27">
+      <c r="B16" s="1">
+        <v>10</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="27">
+      <c r="B17" s="1">
+        <v>11</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6">
-      <c r="B11" s="1">
-        <v>8</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6">
-      <c r="B12" s="1">
-        <v>9</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="27">
-      <c r="B13" s="1">
-        <v>10</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="27">
-      <c r="B14" s="1">
-        <v>11</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="27">
-      <c r="B15" s="1">
-        <v>12</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="27">
-      <c r="B16" s="1">
-        <v>13</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6">
-      <c r="B17" s="1">
-        <v>14</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
@@ -701,13 +731,13 @@
     </row>
     <row r="18" spans="2:6" ht="27">
       <c r="B18" s="1">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F18" s="1">
         <v>1</v>
@@ -715,33 +745,27 @@
     </row>
     <row r="19" spans="2:6" ht="27">
       <c r="B19" s="1">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="1">
         <v>14</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="40.5">
-      <c r="B20" s="1">
-        <v>17</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F20" s="1">
         <v>1</v>
@@ -749,182 +773,304 @@
     </row>
     <row r="21" spans="2:6" ht="27">
       <c r="B21" s="1">
+        <v>15</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="27">
+      <c r="C22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="27">
+      <c r="C23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="40.5">
+      <c r="B24" s="1">
+        <v>17</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="27">
+      <c r="C25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="27">
+      <c r="C26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="27">
+      <c r="B27" s="1">
         <v>18</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="27">
-      <c r="B22" s="1">
+      <c r="C27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="27">
+      <c r="B28" s="1">
         <v>19</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" ht="27">
-      <c r="B23" s="1">
+      <c r="C28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="27">
+      <c r="B29" s="1">
         <v>20</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F23" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" ht="27">
-      <c r="B24" s="1">
+      <c r="C29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="27">
+      <c r="B30" s="1">
         <v>21</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" ht="30">
-      <c r="B25" s="1">
-        <v>22</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="1" t="s">
+      <c r="C30" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" ht="30">
-      <c r="B26" s="1">
-        <v>23</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" ht="30">
-      <c r="B27" s="1">
-        <v>24</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" ht="30">
-      <c r="B28" s="1">
-        <v>25</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" ht="30">
-      <c r="B29" s="1">
-        <v>26</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" ht="30">
-      <c r="B30" s="1">
+      <c r="D30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>33</v>
+      <c r="F30" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:6" ht="30">
       <c r="B31" s="1">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:6" ht="30">
       <c r="B32" s="1">
+        <v>23</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" ht="30">
+      <c r="B33" s="1">
+        <v>24</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="30">
+      <c r="B34" s="1">
+        <v>25</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="30">
+      <c r="B35" s="1">
+        <v>26</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" ht="30">
+      <c r="B36" s="1">
+        <v>27</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" ht="30">
+      <c r="B37" s="1">
+        <v>28</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F37" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" ht="30">
+      <c r="B38" s="1">
         <v>29</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>33</v>
+      <c r="C38" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F38" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" ht="30">
+      <c r="C39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F39" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>